<commit_message>
Update thesis files including new datasets, figures, and documentation
</commit_message>
<xml_diff>
--- a/Datasets/ExperimentTwoFullData.xlsx
+++ b/Datasets/ExperimentTwoFullData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\Uni work\Masters\quarto_manuscript_planaria\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/fordefr_staff_vuw_ac_nz1/Documents/CBNS thesis research/Quarto manuscript/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB808B0-1B3B-4DC1-8F20-E46C6AE76E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="1" xr2:uid="{DB3CF89B-F287-4BB4-9319-FB7C042D6FA6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DB3CF89B-F287-4BB4-9319-FB7C042D6FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="1" r:id="rId1"/>
@@ -14805,10 +14805,10 @@
   <dimension ref="A1:CR71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI1" sqref="AI1"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -15161,7 +15161,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -15458,7 +15458,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A3" s="36">
         <v>2</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>3</v>
       </c>
@@ -16046,7 +16046,7 @@
         <v xml:space="preserve">Day4 Day5 </v>
       </c>
     </row>
-    <row r="5" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A5" s="38">
         <v>4</v>
       </c>
@@ -16337,7 +16337,7 @@
         <v xml:space="preserve">Day2 Day4 Day5 </v>
       </c>
     </row>
-    <row r="6" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A6" s="36">
         <v>5</v>
       </c>
@@ -16628,7 +16628,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A7" s="36">
         <v>6</v>
       </c>
@@ -16919,7 +16919,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A8" s="36">
         <v>7</v>
       </c>
@@ -17210,7 +17210,7 @@
         <v xml:space="preserve">Day1 </v>
       </c>
     </row>
-    <row r="9" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A9" s="36">
         <v>8</v>
       </c>
@@ -17501,7 +17501,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>9</v>
       </c>
@@ -17792,7 +17792,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A11" s="36">
         <v>10</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>11</v>
       </c>
@@ -18374,7 +18374,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A13" s="36">
         <v>12</v>
       </c>
@@ -18665,7 +18665,7 @@
         <v xml:space="preserve">Day1 Day3 </v>
       </c>
     </row>
-    <row r="14" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A14" s="36">
         <v>13</v>
       </c>
@@ -18956,7 +18956,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A15" s="38">
         <v>14</v>
       </c>
@@ -19247,7 +19247,7 @@
         <v xml:space="preserve">Day1 Day2 Day5 </v>
       </c>
     </row>
-    <row r="16" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A16" s="36">
         <v>15</v>
       </c>
@@ -19538,7 +19538,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A17" s="36">
         <v>16</v>
       </c>
@@ -19829,7 +19829,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A18" s="36">
         <v>17</v>
       </c>
@@ -20120,7 +20120,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A19" s="36">
         <v>18</v>
       </c>
@@ -20411,7 +20411,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A20" s="36">
         <v>19</v>
       </c>
@@ -20702,7 +20702,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A21" s="36">
         <v>20</v>
       </c>
@@ -20993,7 +20993,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A22" s="36">
         <v>21</v>
       </c>
@@ -21284,7 +21284,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:96" s="25" customFormat="1" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:96" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="38">
         <v>22</v>
       </c>
@@ -21580,7 +21580,7 @@
       </c>
       <c r="CR23"/>
     </row>
-    <row r="24" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A24" s="36">
         <v>23</v>
       </c>
@@ -21871,7 +21871,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="36">
         <v>24</v>
       </c>
@@ -22162,7 +22162,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A26" s="36">
         <v>25</v>
       </c>
@@ -22453,7 +22453,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A27" s="36">
         <v>26</v>
       </c>
@@ -22744,7 +22744,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A28" s="38">
         <v>27</v>
       </c>
@@ -23035,7 +23035,7 @@
         <v xml:space="preserve">Day2 Day3 Day5 </v>
       </c>
     </row>
-    <row r="29" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A29" s="36">
         <v>28</v>
       </c>
@@ -23326,7 +23326,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>29</v>
       </c>
@@ -23617,7 +23617,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
         <v>30</v>
       </c>
@@ -23908,7 +23908,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
         <v>31</v>
       </c>
@@ -24199,7 +24199,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
         <v>32</v>
       </c>
@@ -24490,7 +24490,7 @@
         <v xml:space="preserve">Day4 </v>
       </c>
     </row>
-    <row r="34" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>33</v>
       </c>
@@ -24781,7 +24781,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A35" s="36">
         <v>34</v>
       </c>
@@ -25072,7 +25072,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:96" s="25" customFormat="1" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:96" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="38">
         <v>35</v>
       </c>
@@ -25368,7 +25368,7 @@
       </c>
       <c r="CR36"/>
     </row>
-    <row r="37" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A37" s="36">
         <v>36</v>
       </c>
@@ -25659,7 +25659,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A38" s="36">
         <v>37</v>
       </c>
@@ -25950,7 +25950,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A39" s="36">
         <v>38</v>
       </c>
@@ -26241,7 +26241,7 @@
         <v xml:space="preserve">Day1 </v>
       </c>
     </row>
-    <row r="40" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A40" s="36">
         <v>39</v>
       </c>
@@ -26532,7 +26532,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A41" s="38">
         <v>40</v>
       </c>
@@ -26823,7 +26823,7 @@
         <v xml:space="preserve">Day5 </v>
       </c>
     </row>
-    <row r="42" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A42" s="36">
         <v>41</v>
       </c>
@@ -27114,7 +27114,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A43" s="36">
         <v>42</v>
       </c>
@@ -27405,7 +27405,7 @@
         <v xml:space="preserve">Day2 </v>
       </c>
     </row>
-    <row r="44" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A44" s="36">
         <v>43</v>
       </c>
@@ -27696,7 +27696,7 @@
         <v xml:space="preserve">Day3 </v>
       </c>
     </row>
-    <row r="45" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A45" s="38">
         <v>44</v>
       </c>
@@ -27991,7 +27991,7 @@
         <v xml:space="preserve">Day2 Day3 </v>
       </c>
     </row>
-    <row r="46" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A46" s="36">
         <v>45</v>
       </c>
@@ -28282,7 +28282,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A47" s="36">
         <v>46</v>
       </c>
@@ -28573,7 +28573,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:96" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A48" s="38">
         <v>47</v>
       </c>
@@ -28864,7 +28864,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A49" s="36">
         <v>48</v>
       </c>
@@ -29155,7 +29155,7 @@
         <v xml:space="preserve">Day1 Day3 </v>
       </c>
     </row>
-    <row r="50" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A50" s="36">
         <v>49</v>
       </c>
@@ -29446,7 +29446,7 @@
         <v xml:space="preserve">Day1 </v>
       </c>
     </row>
-    <row r="51" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A51" s="38">
         <v>50</v>
       </c>
@@ -29737,7 +29737,7 @@
         <v xml:space="preserve">Day1 Day2 </v>
       </c>
     </row>
-    <row r="52" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A52" s="36">
         <v>51</v>
       </c>
@@ -30028,7 +30028,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A53" s="38">
         <v>52</v>
       </c>
@@ -30319,7 +30319,7 @@
         <v xml:space="preserve">Day1 Day5 </v>
       </c>
     </row>
-    <row r="54" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A54" s="36">
         <v>53</v>
       </c>
@@ -30610,7 +30610,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A55" s="36">
         <v>54</v>
       </c>
@@ -30901,7 +30901,7 @@
         <v xml:space="preserve">Day1 </v>
       </c>
     </row>
-    <row r="56" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A56" s="38">
         <v>55</v>
       </c>
@@ -31192,7 +31192,7 @@
         <v xml:space="preserve">Day2 Day5 </v>
       </c>
     </row>
-    <row r="57" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A57" s="38">
         <v>56</v>
       </c>
@@ -31483,7 +31483,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A58" s="36">
         <v>57</v>
       </c>
@@ -31774,7 +31774,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A59" s="36">
         <v>58</v>
       </c>
@@ -32065,7 +32065,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A60" s="36">
         <v>59</v>
       </c>
@@ -32356,7 +32356,7 @@
         <v xml:space="preserve">Day3 </v>
       </c>
     </row>
-    <row r="61" spans="1:94" ht="21.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A61" s="36">
         <v>60</v>
       </c>

</xml_diff>